<commit_message>
Final Version V1- Added the top companies in each sector with sum of funds received
</commit_message>
<xml_diff>
--- a/Data/Investments.xlsx
+++ b/Data/Investments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahima.prasad.UPGRAD\Desktop\Random\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Masters\EDA_SprakFunds_Assignment\EDA_SparkFunds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BDF173-077C-4F99-8E81-F85A762DC751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DBB96E-D825-4E49-BCD6-05AA65CB5B71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="1860" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -26,15 +26,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t>C1</t>
   </si>
@@ -358,13 +355,61 @@
   </si>
   <si>
     <t>Representative funding amount of private equity type</t>
+  </si>
+  <si>
+    <t>permalink</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>venture</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>GBR (United Kingdom)</t>
+  </si>
+  <si>
+    <t>IND (India)</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleantech / Semiconductors </t>
+  </si>
+  <si>
+    <t xml:space="preserve">News, Search and Messaging </t>
+  </si>
+  <si>
+    <t>Social, Finance, Analytics, Advertising</t>
+  </si>
+  <si>
+    <t>virtustream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electric-cloud </t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstcry-com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">shotspotter </t>
+  </si>
+  <si>
+    <t>eusa-pharma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manthan-systems </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,6 +477,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -574,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -642,6 +693,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -992,7 +1044,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,23 +1055,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="26"/>
       <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1039,7 +1091,9 @@
       <c r="B5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="17">
+        <v>90247</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -1048,7 +1102,9 @@
       <c r="B6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="17">
+        <v>66368</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -1057,7 +1113,9 @@
       <c r="B7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="17" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -1066,7 +1124,9 @@
       <c r="B8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="17" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -1075,7 +1135,9 @@
       <c r="B9" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="17">
+        <v>114942</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="11"/>
@@ -1099,6 +1161,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1107,7 +1170,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,21 +1181,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
     </row>
     <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1152,7 +1215,9 @@
       <c r="B5" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12">
+        <v>5000000</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
@@ -1161,7 +1226,9 @@
       <c r="B6" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="12">
+        <v>414906</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
@@ -1170,7 +1237,9 @@
       <c r="B7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="12">
+        <v>300000</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
@@ -1179,7 +1248,9 @@
       <c r="B8" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="12">
+        <v>20000000</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
@@ -1188,7 +1259,9 @@
       <c r="B9" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1215,7 +1288,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,21 +1299,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -1260,7 +1333,9 @@
       <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
@@ -1269,7 +1344,9 @@
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -1278,7 +1355,9 @@
       <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1303,8 +1382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,23 +1396,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="32"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="34"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
@@ -1359,9 +1438,15 @@
       <c r="B5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
+      <c r="C5" s="17">
+        <v>11945</v>
+      </c>
+      <c r="D5" s="17">
+        <v>611</v>
+      </c>
+      <c r="E5" s="17">
+        <v>327</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
@@ -1370,9 +1455,15 @@
       <c r="B6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="C6" s="17">
+        <v>106710641155</v>
+      </c>
+      <c r="D6" s="17">
+        <v>5289424747</v>
+      </c>
+      <c r="E6" s="17">
+        <v>2943543602</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
@@ -1381,9 +1472,15 @@
       <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="C7" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
@@ -1392,9 +1489,15 @@
       <c r="B8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
+      <c r="C8" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
@@ -1403,9 +1506,15 @@
       <c r="B9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
+      <c r="C9" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
@@ -1414,9 +1523,15 @@
       <c r="B10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="C10" s="25">
+        <v>2923</v>
+      </c>
+      <c r="D10" s="17">
+        <v>143</v>
+      </c>
+      <c r="E10" s="17">
+        <v>109</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
@@ -1425,9 +1540,15 @@
       <c r="B11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="C11" s="25">
+        <v>2658</v>
+      </c>
+      <c r="D11" s="17">
+        <v>130</v>
+      </c>
+      <c r="E11" s="17">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
@@ -1436,9 +1557,15 @@
       <c r="B12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="C12" s="25">
+        <v>2347</v>
+      </c>
+      <c r="D12" s="17">
+        <v>129</v>
+      </c>
+      <c r="E12" s="17">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
@@ -1447,9 +1574,15 @@
       <c r="B13" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="C13" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
@@ -1458,9 +1591,15 @@
       <c r="B14" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="C14" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1468,7 +1607,7 @@
     <mergeCell ref="A3:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="B5">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1476,7 +1615,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1487,8 +1626,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:E14">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="A5:E7 A9:E9 A8:C8 A13:E14 A10:B12 D10:E12 E8:E9">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1500,7 +1639,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A14">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1509,6 +1648,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
changed the second top in GBR
</commit_message>
<xml_diff>
--- a/Data/Investments.xlsx
+++ b/Data/Investments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Masters\EDA_SprakFunds_Assignment\EDA_SparkFunds\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DBB96E-D825-4E49-BCD6-05AA65CB5B71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E684C9-D56E-431A-8DE4-B85BA60B686E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="1860" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-6300" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -33,15 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
     <t>Sl.no</t>
   </si>
   <si>
@@ -399,10 +390,19 @@
     <t xml:space="preserve">shotspotter </t>
   </si>
   <si>
-    <t>eusa-pharma</t>
-  </si>
-  <si>
     <t xml:space="preserve">manthan-systems </t>
+  </si>
+  <si>
+    <t>celltick-technologies</t>
+  </si>
+  <si>
+    <t>C1(USA)</t>
+  </si>
+  <si>
+    <t>C2(GBR)</t>
+  </si>
+  <si>
+    <t>C3(IND)</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -1056,7 +1056,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="15"/>
@@ -1068,20 +1068,20 @@
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1089,7 +1089,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" s="17">
         <v>90247</v>
@@ -1100,7 +1100,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" s="17">
         <v>66368</v>
@@ -1111,10 +1111,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1122,10 +1122,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.25">
@@ -1133,7 +1133,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" s="17">
         <v>114942</v>
@@ -1182,7 +1182,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B1" s="28"/>
     </row>
@@ -1192,20 +1192,20 @@
     </row>
     <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1213,7 +1213,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C5" s="12">
         <v>5000000</v>
@@ -1224,7 +1224,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C6" s="12">
         <v>414906</v>
@@ -1235,7 +1235,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" s="12">
         <v>300000</v>
@@ -1246,7 +1246,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C8" s="12">
         <v>20000000</v>
@@ -1257,10 +1257,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1300,7 +1300,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B1" s="28"/>
     </row>
@@ -1310,20 +1310,20 @@
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
@@ -1331,10 +1331,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
@@ -1342,10 +1342,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
@@ -1353,10 +1353,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1382,8 +1382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,7 +1397,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B1" s="32"/>
     </row>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
@@ -1416,19 +1416,19 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1436,7 +1436,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5" s="17">
         <v>11945</v>
@@ -1453,7 +1453,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C6" s="17">
         <v>106710641155</v>
@@ -1470,16 +1470,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1487,16 +1487,16 @@
         <v>4</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1504,16 +1504,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1521,7 +1521,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C10" s="25">
         <v>2923</v>
@@ -1538,7 +1538,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C11" s="25">
         <v>2658</v>
@@ -1555,7 +1555,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C12" s="25">
         <v>2347</v>
@@ -1572,16 +1572,16 @@
         <v>9</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1589,16 +1589,16 @@
         <v>10</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>